<commit_message>
refactor some vibe code
</commit_message>
<xml_diff>
--- a/sample_data/comment-list.xlsx
+++ b/sample_data/comment-list.xlsx
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>8</v>
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
         <v>8</v>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
         <v>8</v>
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
         <v>8</v>
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
         <v>8</v>
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
         <v>8</v>
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
         <v>8</v>
@@ -1006,7 +1006,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
         <v>8</v>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
         <v>8</v>
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
         <v>8</v>
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
         <v>8</v>
@@ -1234,7 +1234,7 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
         <v>8</v>
@@ -1291,7 +1291,7 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="L14" t="n">
         <v>8</v>
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
         <v>8</v>
@@ -1405,7 +1405,7 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
         <v>8</v>
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
         <v>8</v>
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
         <v>8</v>
@@ -1576,7 +1576,7 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
         <v>8</v>
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
         <v>8</v>
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="K21" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
         <v>8</v>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
         <v>8</v>
@@ -1804,7 +1804,7 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="L23" t="n">
         <v>8</v>
@@ -1861,7 +1861,7 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
         <v>8</v>
@@ -1918,7 +1918,7 @@
         </is>
       </c>
       <c r="K25" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="L25" t="n">
         <v>8</v>
@@ -1975,7 +1975,7 @@
         </is>
       </c>
       <c r="K26" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="L26" t="n">
         <v>9</v>
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="K27" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
         <v>9</v>

</xml_diff>